<commit_message>
Add additional user credentials to Postman CSV and update Skills.xlsx
</commit_message>
<xml_diff>
--- a/10 Resume/Skills.xlsx
+++ b/10 Resume/Skills.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Working\GitHub\Aptech\aptech-tester\10. Resume\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tony/GitHub/Aptech/tester-tutorials/10 Resume/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59A8D5D8-7B13-4FD2-838C-6F4105516DB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0859EBA4-0FC2-9349-A48A-86E415E85E4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="38700" windowHeight="15345" xr2:uid="{B5F4DA4E-4B18-4F7B-BA47-1584F7837A0A}"/>
+    <workbookView xWindow="100" yWindow="920" windowWidth="34560" windowHeight="19580" xr2:uid="{B5F4DA4E-4B18-4F7B-BA47-1584F7837A0A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="46">
   <si>
     <t>DATABASE</t>
   </si>
@@ -120,9 +120,6 @@
     <t>Nắm bản chất TEST HỒI QUY và quy trình thực hiện</t>
   </si>
   <si>
-    <t>Nắm bản chất kỹ Static Testing và Dynamic Testing</t>
-  </si>
-  <si>
     <t>Nắm bản chất Black Box Test</t>
   </si>
   <si>
@@ -172,6 +169,12 @@
   </si>
   <si>
     <t>H</t>
+  </si>
+  <si>
+    <t>Nắm bản chất kỹ thuật Static Testing và Dynamic Testing</t>
+  </si>
+  <si>
+    <t>Viết các scripts để test hồi quy &amp; tự động</t>
   </si>
 </sst>
 </file>
@@ -266,7 +269,7 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>56</xdr:row>
+      <xdr:row>57</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="152400" cy="152400"/>
@@ -322,9 +325,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -362,7 +365,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -468,7 +471,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -610,7 +613,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -618,28 +621,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{829EBD80-163A-49A3-AF11-33FB8948D068}">
-  <dimension ref="A1:E62"/>
+  <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27" style="2" customWidth="1"/>
-    <col min="3" max="3" width="142.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="2"/>
-    <col min="5" max="5" width="98.7109375" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="2"/>
+    <col min="3" max="3" width="142.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.1640625" style="2"/>
+    <col min="5" max="5" width="98.6640625" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="9.1640625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -669,12 +672,12 @@
     <row r="6" spans="1:3">
       <c r="B6" s="1"/>
       <c r="C6" s="2" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="C7" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -683,53 +686,53 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" ht="18">
       <c r="C9" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" ht="18">
       <c r="C10" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" ht="18">
       <c r="C11" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" ht="18">
       <c r="C12" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="4"/>
+    </row>
+    <row r="14" spans="1:3" ht="18">
+      <c r="C14" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="18">
+      <c r="C15" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="4"/>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="C14" s="4" t="s">
+    </row>
+    <row r="16" spans="1:3" ht="18">
+      <c r="C16" s="4" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="C15" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="C16" s="4" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>0</v>
@@ -761,14 +764,14 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E22" s="4"/>
     </row>
-    <row r="23" spans="1:5" ht="51.75">
+    <row r="23" spans="1:5" ht="54">
       <c r="C23" s="6" t="s">
         <v>9</v>
       </c>
@@ -782,101 +785,104 @@
     </row>
     <row r="25" spans="1:5">
       <c r="C25" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E25" s="4"/>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="C26" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E25" s="4"/>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B26" s="1" t="s">
+      <c r="E26" s="4"/>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="E26" s="4"/>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="C27" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="E27" s="4"/>
     </row>
     <row r="28" spans="1:5">
       <c r="C28" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E28" s="4"/>
     </row>
     <row r="29" spans="1:5">
       <c r="C29" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E29" s="4"/>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="C30" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E29" s="4"/>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B30" s="1" t="s">
+      <c r="E30" s="4"/>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="E30" s="4"/>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="C31" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="E31" s="4"/>
     </row>
     <row r="32" spans="1:5">
       <c r="C32" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E32" s="4"/>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="C33" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E32" s="4"/>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="C33" s="5" t="s">
+      <c r="E33" s="4"/>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="C34" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
-      <c r="C34" s="2" t="s">
+    <row r="35" spans="1:5">
+      <c r="C35" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
-      <c r="A35" s="1" t="s">
+    <row r="36" spans="1:5">
+      <c r="A36" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="C37" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="C38" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B39" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
-      <c r="C36" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="C37" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B38" s="1" t="s">
+    <row r="40" spans="1:5">
+      <c r="C40" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="C39" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="50" spans="5:5">
-      <c r="E50" s="4"/>
     </row>
     <row r="51" spans="5:5">
       <c r="E51" s="4"/>
@@ -913,6 +919,9 @@
     </row>
     <row r="62" spans="5:5">
       <c r="E62" s="4"/>
+    </row>
+    <row r="63" spans="5:5">
+      <c r="E63" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>